<commit_message>
Aggiunti dettagli nella colonna gestione Errore
ID 31, 39, 75, 76, 77, 78, 79, 80, 81, 82, 83,  84, 85, 93, la procedura di gestione dell’errore e le modalità di invio del documento al FSE a seguito della risoluzione dell’errore.
ID 47, la modalità con cui viene gestito il caso di timeout, indicando se il documento viene messo in una coda che si occupa di eseguire la retry o se invece l'operazione di retry viene eseguita manualmente dall’operatore in back office.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGR/2023.04.01.1200/report-checklist.xlsx
+++ b/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGR/2023.04.01.1200/report-checklist.xlsx
@@ -1441,8 +1441,126 @@
     <t>2023-05-08T13:27:00Z</t>
   </si>
   <si>
-    <t xml:space="preserve">
-    "type": "/msg/jwt-validation",
+    <t>c0b50b2009b80b95</t>
+  </si>
+  <si>
+    <t>2023-05-08T13:36:14Z</t>
+  </si>
+  <si>
+    <t>2023-05-08T13:50:53Z</t>
+  </si>
+  <si>
+    <t>90038ac2c3df540b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.f74a8b7dcc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:15:42Z</t>
+  </si>
+  <si>
+    <t>72a67d9e159868a6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.9a6c362fad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:20:40Z</t>
+  </si>
+  <si>
+    <t>8b2418aeec90dfb6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.574e50dd0c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:34:40Z</t>
+  </si>
+  <si>
+    <t>172e169bb94c20be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.a559d74b1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:37:19Z</t>
+  </si>
+  <si>
+    <t>d13e1271ac33342a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.bba3c01a95^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:42:05Z</t>
+  </si>
+  <si>
+    <t>87e788cdab44657a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.d96e7bd7ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>29fa4fe8ef74407f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.d3328ca423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-08T14:52:51Z</t>
+  </si>
+  <si>
+    <t>005a28436c841505</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.50303d6c67^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "title": "Errore semantico.",
+    "detail": "[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
+  </si>
+  <si>
+    <t>2023-05-09T06:33:46Z</t>
+  </si>
+  <si>
+    <t>67f1ce78b0c023b8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.343070c8f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
+   </t>
+  </si>
+  <si>
+    <t>2023-05-09T06:39:17Z</t>
+  </si>
+  <si>
+    <t>2fcf2c5d49644b11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.84a34c6a05^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
+    </t>
+  </si>
+  <si>
+    <t>2023-05-09T06:48:41Z</t>
+  </si>
+  <si>
+    <t>3cf72965a4e2699f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.8e0e30c9b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
+    </t>
+  </si>
+  <si>
+    <t>2023-05-09T06:51:15Z</t>
+  </si>
+  <si>
+    <t>1307baffc71e63ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.1ace433aca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
+    </t>
+  </si>
+  <si>
+    <t>Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.    "type": "/msg/jwt-validation",
     "title": "Campo token JWT non valido.",
     "detail": "Il campo action_id non è valorizzato",
     "status": 403,
@@ -1450,7 +1568,7 @@
     "workflowInstanceId": "UNKNOWN_WORKFLOW_ID"</t>
   </si>
   <si>
-    <t xml:space="preserve">
+    <t>Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.
     "type": "/msg/jwt-validation",
     "title": "Campo token JWT non valido.",
     "detail": "Il campo purpose_of_use non è corretto",
@@ -1460,175 +1578,56 @@
     "govway_id": null</t>
   </si>
   <si>
-    <t>c0b50b2009b80b95</t>
-  </si>
-  <si>
-    <t>2023-05-08T13:36:14Z</t>
-  </si>
-  <si>
-    <t>Errore : Timeout dell'operazione.</t>
-  </si>
-  <si>
-    <t>2023-05-08T13:50:53Z</t>
-  </si>
-  <si>
-    <t>90038ac2c3df540b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.f74a8b7dcc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore di sintassi.",
+    <t>Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.Errore : Timeout dell'operazione.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente. "title": "Errore di sintassi.",
     "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected."</t>
   </si>
   <si>
-    <t>2023-05-08T14:15:42Z</t>
-  </si>
-  <si>
-    <t>72a67d9e159868a6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.9a6c362fad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   "title": "Errore semantico.",
+    <t xml:space="preserve">Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.   "title": "Errore semantico.",
     "detail": "[Errore-46| codice fiscale 'PROVAX00x00x0x' cittadino ed operatore: 16 cifre [A-Z0-9]{16}],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']",
  </t>
   </si>
   <si>
-    <t>2023-05-08T14:20:40Z</t>
-  </si>
-  <si>
-    <t>8b2418aeec90dfb6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.574e50dd0c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore semantico.",
+    <t xml:space="preserve">    Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente."title": "Errore semantico.",
     "detail": "[ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code  valorizzato con 'N' o 'V', e il suo @codeSystem  con '2.16.840.1.113883.5.25'],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
   <si>
-    <t>2023-05-08T14:34:40Z</t>
-  </si>
-  <si>
-    <t>172e169bb94c20be</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.a559d74b1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   "title": "Errore semantico.",
+    <t xml:space="preserve">   Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente."title": "Errore semantico.",
     "detail": "[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.   ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']",</t>
   </si>
   <si>
-    <t>2023-05-08T14:37:19Z</t>
-  </si>
-  <si>
-    <t>d13e1271ac33342a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.bba3c01a95^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   "title": "Errore semantico.",
+    <t xml:space="preserve">  Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente. "title": "Errore semantico.",
     "detail": "[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']",</t>
   </si>
   <si>
-    <t>2023-05-08T14:42:05Z</t>
-  </si>
-  <si>
-    <t>87e788cdab44657a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.d96e7bd7ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore vocabolario.",
+    <t xml:space="preserve">Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.    "title": "Errore vocabolario.",
     "detail": "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]",
  </t>
   </si>
   <si>
-    <t>29fa4fe8ef74407f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.d3328ca423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-08T14:52:51Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore semantico.",
+    <t xml:space="preserve">    Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente."title": "Errore semantico.",
     "detail": "[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
   <si>
-    <t>005a28436c841505</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.50303d6c67^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore semantico.",
-    "detail": "[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
-  </si>
-  <si>
-    <t>2023-05-09T06:33:46Z</t>
-  </si>
-  <si>
-    <t>67f1ce78b0c023b8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore di sintassi.",
+    <t xml:space="preserve">Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente."title": "Errore di sintassi.",
+    "detail": "ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.",
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.  "title": "Errore di sintassi.",
     "detail": "ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'extension' on element 'id' is not valid with respect to its type, 'st'.",
  </t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.343070c8f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
-   </t>
-  </si>
-  <si>
-    <t>2023-05-09T06:39:17Z</t>
-  </si>
-  <si>
-    <t>2fcf2c5d49644b11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.84a34c6a05^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
-    </t>
-  </si>
-  <si>
-    <t>2023-05-09T06:48:41Z</t>
-  </si>
-  <si>
-    <t>3cf72965a4e2699f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.8e0e30c9b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "title": "Errore semantico.",
-    "detail": "[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']</t>
-  </si>
-  <si>
-    <t>2023-05-09T06:51:15Z</t>
-  </si>
-  <si>
-    <t>1307baffc71e63ed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.160112.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.1ace433aca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"title": "Errore di sintassi.",
+    <t xml:space="preserve">Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente."title": "Errore di sintassi.",
     "detail": "ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element 'component' is not complete. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":section}' is expected.",
    </t>
   </si>
   <si>
-    <t xml:space="preserve">"title": "Errore di sintassi.",
-    "detail": "ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.",
-</t>
+    <t>Viene gestito in back office ed un operatore rieseguirà l'operazione manualmente.    "title": "Errore semantico.",
+    "detail": "[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']</t>
   </si>
 </sst>
 </file>
@@ -3546,10 +3545,10 @@
   <dimension ref="A1:O991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="G93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L92" sqref="L92"/>
+      <selection pane="bottomRight" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4518,7 +4517,7 @@
         <v>91</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>329</v>
+        <v>367</v>
       </c>
       <c r="K36" s="19" t="s">
         <v>51</v>
@@ -4697,16 +4696,16 @@
         <v>45054</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I42" s="18" t="s">
         <v>91</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>330</v>
+        <v>368</v>
       </c>
       <c r="K42" s="19" t="s">
         <v>51</v>
@@ -4888,7 +4887,7 @@
       <c r="H48" s="18"/>
       <c r="I48" s="18"/>
       <c r="J48" s="19" t="s">
-        <v>333</v>
+        <v>369</v>
       </c>
       <c r="K48" s="19" t="s">
         <v>51</v>
@@ -5676,16 +5675,16 @@
         <v>45054</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="J75" s="19" t="s">
-        <v>337</v>
+        <v>370</v>
       </c>
       <c r="K75" s="19" t="s">
         <v>51</v>
@@ -5719,16 +5718,16 @@
         <v>45054</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J76" s="19" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
       <c r="K76" s="19" t="s">
         <v>51</v>
@@ -5762,16 +5761,16 @@
         <v>45054</v>
       </c>
       <c r="G77" s="18" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H77" s="18" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="J77" s="19" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="K77" s="19" t="s">
         <v>51</v>
@@ -5805,16 +5804,16 @@
         <v>45054</v>
       </c>
       <c r="G78" s="18" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H78" s="18" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="J78" s="19" t="s">
-        <v>349</v>
+        <v>373</v>
       </c>
       <c r="K78" s="19" t="s">
         <v>51</v>
@@ -5848,16 +5847,16 @@
         <v>45054</v>
       </c>
       <c r="G79" s="18" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="H79" s="18" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="J79" s="19" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="K79" s="19" t="s">
         <v>51</v>
@@ -5891,16 +5890,16 @@
         <v>45054</v>
       </c>
       <c r="G80" s="18" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H80" s="18" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="J80" s="19" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="K80" s="19" t="s">
         <v>51</v>
@@ -5934,16 +5933,16 @@
         <v>45054</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="H81" s="18" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="J81" s="19" t="s">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="K81" s="19" t="s">
         <v>51</v>
@@ -5977,16 +5976,16 @@
         <v>45054</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="H82" s="18" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="J82" s="19" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="K82" s="19" t="s">
         <v>51</v>
@@ -6020,16 +6019,16 @@
         <v>45055</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="J83" s="19" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="K83" s="19" t="s">
         <v>51</v>
@@ -6063,16 +6062,16 @@
         <v>45055</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="J84" s="19" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="K84" s="19" t="s">
         <v>51</v>
@@ -6106,13 +6105,13 @@
         <v>45055</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="J85" s="19" t="s">
         <v>379</v>
@@ -6380,16 +6379,16 @@
         <v>45055</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="J93" s="19" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="K93" s="19" t="s">
         <v>51</v>

</xml_diff>